<commit_message>
MPTrx - template updates, make it compile in refactor branch
</commit_message>
<xml_diff>
--- a/MPTrx/_Parcel Transportation.xlsx
+++ b/MPTrx/_Parcel Transportation.xlsx
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="74">
   <si>
     <t>Scope</t>
   </si>
@@ -96,9 +96,6 @@
     <t>TTPhrase</t>
   </si>
   <si>
-    <t>[Organization,]</t>
-  </si>
-  <si>
     <t>[TParties]</t>
   </si>
   <si>
@@ -115,9 +112,6 @@
   </si>
   <si>
     <t>Transporter</t>
-  </si>
-  <si>
-    <t>PostNL, DHL, DPD, TNT</t>
   </si>
   <si>
     <t>Party that requests a parcel to be transported</t>
@@ -764,24 +758,24 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" t="s">
         <v>28</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="C3" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -792,10 +786,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="F1" sqref="F1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -805,16 +799,15 @@
     <col min="3" max="3" width="10.33203125" style="13" customWidth="1"/>
     <col min="4" max="4" width="15.44140625" style="13" customWidth="1"/>
     <col min="5" max="5" width="41.109375" customWidth="1"/>
-    <col min="6" max="6" width="25.109375" style="13" customWidth="1"/>
-    <col min="7" max="7" width="10.44140625" style="13" customWidth="1"/>
+    <col min="6" max="9" width="14.77734375" style="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C1" s="15" t="s">
         <v>8</v>
@@ -823,14 +816,22 @@
         <v>9</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" s="6"/>
-    </row>
-    <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -848,11 +849,19 @@
         <v>13</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="6"/>
-    </row>
-    <row r="3" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="str">
         <f>IF(OR($C3="",$D3=""),"",CONCATENATE("SHR_",$C3,"_",$D3))</f>
         <v>SHR_PclTxTplt_Sender</v>
@@ -866,15 +875,17 @@
         <v>PclTxTplt</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
-    </row>
-    <row r="4" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+    </row>
+    <row r="4" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="str">
         <f>IF(OR($C4="",$D4=""),"",CONCATENATE("SHR_",$C4,"_",$D4))</f>
         <v>SHR_PclTxTplt_Transporter</v>
@@ -888,17 +899,25 @@
         <v>PclTxTplt</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" s="13"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="str">
         <f t="shared" ref="A5" si="1">IF(OR($C5="",$D5=""),"",CONCATENATE("SHR_",$C5,"_",$D5))</f>
         <v/>
@@ -916,7 +935,7 @@
       <c r="F5" s="7"/>
       <c r="G5" s="8"/>
     </row>
-    <row r="7" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="str">
         <f>IF(OR($C7="",$D7=""),"",CONCATENATE("SHR_",$C7,"_",$D7))</f>
         <v>SHR_PclRxTplt_Transporter</v>
@@ -930,17 +949,25 @@
         <v>PclRxTplt</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" s="7"/>
-    </row>
-    <row r="8" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="str">
         <f t="shared" ref="A8:A9" si="3">IF(OR($C8="",$D8=""),"",CONCATENATE("SHR_",$C8,"_",$D8))</f>
         <v>SHR_PclRxTplt_Recipient</v>
@@ -954,15 +981,17 @@
         <v>PclRxTplt</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="13"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -1005,10 +1034,10 @@
   <sheetData>
     <row r="1" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="22" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C1" s="15" t="s">
         <v>8</v>
@@ -1017,7 +1046,7 @@
         <v>9</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F1" s="9" t="s">
         <v>11</v>
@@ -1058,13 +1087,13 @@
         <v>PclTxTplt</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -1081,13 +1110,13 @@
         <v>PclTxTplt</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -1104,13 +1133,13 @@
         <v>PclTxTplt</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -1127,13 +1156,13 @@
         <v>PclTxTplt</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -1150,13 +1179,13 @@
         <v>PclRxTplt</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -1173,13 +1202,13 @@
         <v>PclRxTplt</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1226,7 +1255,7 @@
         <v>11</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
@@ -1261,7 +1290,7 @@
         <v>13</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
@@ -1289,13 +1318,13 @@
         <v>PclTxTplt</v>
       </c>
       <c r="C3" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="13" t="s">
-        <v>19</v>
-      </c>
       <c r="E3" s="12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F3" s="7"/>
     </row>
@@ -1309,13 +1338,13 @@
         <v>PclTxTplt</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H4" s="7"/>
     </row>
@@ -1329,13 +1358,13 @@
         <v>PclTxTplt</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.3">
@@ -1348,13 +1377,13 @@
         <v>PclTxTplt</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.3">
@@ -1367,13 +1396,13 @@
         <v>PclTxTplt</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
@@ -1388,13 +1417,13 @@
         <v>PclTxTplt</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F8" s="11">
         <v>2</v>
@@ -1412,13 +1441,13 @@
         <v>PclTxTplt</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="J9" s="7"/>
     </row>
@@ -1432,13 +1461,13 @@
         <v>PclTxTplt</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.3">
@@ -1454,13 +1483,13 @@
         <v>PclRxTplt</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E12" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.3">
@@ -1473,13 +1502,13 @@
         <v>PclRxTplt</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.3">
@@ -1492,13 +1521,13 @@
         <v>PclRxTplt</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.3">
@@ -1511,13 +1540,13 @@
         <v>PclRxTplt</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F15" s="11">
         <v>2</v>
@@ -1625,10 +1654,10 @@
   <sheetData>
     <row r="1" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
@@ -1654,10 +1683,10 @@
     </row>
     <row r="2" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
@@ -1683,34 +1712,34 @@
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
MPTrx - starts to run again. Some issues remain, e.g. with html-templates
</commit_message>
<xml_diff>
--- a/MPTrx/_Parcel Transportation.xlsx
+++ b/MPTrx/_Parcel Transportation.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D037EF60-7A84-49E2-ACEB-222641718A53}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{970535DF-F19F-4294-B941-01170BA63400}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-42300" yWindow="1932" windowWidth="17280" windowHeight="9072" tabRatio="703" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="703" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#Scopes" sheetId="1" r:id="rId1"/>
     <sheet name="#TTParties" sheetId="14" r:id="rId2"/>
-    <sheet name="#Concerns" sheetId="19" r:id="rId3"/>
+    <sheet name="#Objectives" sheetId="19" r:id="rId3"/>
     <sheet name="#TTexts" sheetId="6" r:id="rId4"/>
     <sheet name="#Organizations" sheetId="20" r:id="rId5"/>
   </sheets>
@@ -134,12 +134,6 @@
     <t>Weight</t>
   </si>
   <si>
-    <t>PclRxTplt</t>
-  </si>
-  <si>
-    <t>PclTxTplt</t>
-  </si>
-  <si>
     <t>Parcel Transportation - Delivery</t>
   </si>
   <si>
@@ -288,6 +282,12 @@
   </si>
   <si>
     <t>ttIsaTTParty</t>
+  </si>
+  <si>
+    <t>Scope_SendParcelTemplate</t>
+  </si>
+  <si>
+    <t>Scope_DlvrParcelTemplate</t>
   </si>
 </sst>
 </file>
@@ -773,12 +773,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.6640625" style="8" customWidth="1"/>
+    <col min="1" max="1" width="23.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" style="8" customWidth="1"/>
     <col min="3" max="3" width="57.5546875" style="2" customWidth="1"/>
     <col min="4" max="16384" width="8.88671875" style="2"/>
   </cols>
@@ -807,24 +809,24 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" t="s">
         <v>24</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C3" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -837,15 +839,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.33203125" customWidth="1"/>
-    <col min="2" max="2" width="1.21875" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" style="13" customWidth="1"/>
+    <col min="1" max="1" width="38.33203125" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="3" max="3" width="23.77734375" style="13" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.44140625" style="13" customWidth="1"/>
     <col min="5" max="5" width="41.109375" customWidth="1"/>
     <col min="6" max="9" width="20.77734375" style="13" customWidth="1"/>
@@ -853,10 +855,10 @@
   <sheetData>
     <row r="1" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C1" s="15" t="s">
         <v>8</v>
@@ -868,16 +870,16 @@
         <v>14</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -898,30 +900,30 @@
         <v>13</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="str">
         <f>IF(OR($C3="",$D3=""),"",CONCATENATE("SHR_",$C3,"_",$D3))</f>
-        <v>SHR_PclTxTplt_Sender</v>
+        <v>SHR_Scope_SendParcelTemplate_Sender</v>
       </c>
       <c r="B3" s="4" t="str">
         <f>IF($A3="","",$A3)</f>
-        <v>SHR_PclTxTplt_Sender</v>
+        <v>SHR_Scope_SendParcelTemplate_Sender</v>
       </c>
       <c r="C3" s="20" t="str">
         <f>IF($D3="","",'#Scopes'!$A$3)</f>
-        <v>PclTxTplt</v>
+        <v>Scope_SendParcelTemplate</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>16</v>
@@ -937,15 +939,15 @@
     <row r="4" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="str">
         <f>IF(OR($C4="",$D4=""),"",CONCATENATE("SHR_",$C4,"_",$D4))</f>
-        <v>SHR_PclTxTplt_Transporter</v>
+        <v>SHR_Scope_SendParcelTemplate_Transporter</v>
       </c>
       <c r="B4" s="4" t="str">
         <f t="shared" ref="B4:B5" si="0">IF($A4="","",$A4)</f>
-        <v>SHR_PclTxTplt_Transporter</v>
+        <v>SHR_Scope_SendParcelTemplate_Transporter</v>
       </c>
       <c r="C4" s="20" t="str">
         <f>IF($D4="","",'#Scopes'!$A$3)</f>
-        <v>PclTxTplt</v>
+        <v>Scope_SendParcelTemplate</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>17</v>
@@ -954,16 +956,16 @@
         <v>19</v>
       </c>
       <c r="F4" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="G4" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>39</v>
-      </c>
       <c r="I4" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -987,15 +989,15 @@
     <row r="7" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="str">
         <f>IF(OR($C7="",$D7=""),"",CONCATENATE("SHR_",$C7,"_",$D7))</f>
-        <v>SHR_PclRxTplt_Transporter</v>
+        <v>SHR_Scope_DlvrParcelTemplate_Transporter</v>
       </c>
       <c r="B7" s="4" t="str">
         <f t="shared" ref="B7:B9" si="2">IF($A7="","",$A7)</f>
-        <v>SHR_PclRxTplt_Transporter</v>
+        <v>SHR_Scope_DlvrParcelTemplate_Transporter</v>
       </c>
       <c r="C7" s="20" t="str">
         <f>IF($D7="","",'#Scopes'!$A$4)</f>
-        <v>PclRxTplt</v>
+        <v>Scope_DlvrParcelTemplate</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>17</v>
@@ -1004,36 +1006,36 @@
         <v>19</v>
       </c>
       <c r="F7" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="H7" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="G7" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="H7" s="8" t="s">
-        <v>39</v>
-      </c>
       <c r="I7" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="str">
         <f t="shared" ref="A8:A9" si="3">IF(OR($C8="",$D8=""),"",CONCATENATE("SHR_",$C8,"_",$D8))</f>
-        <v>SHR_PclRxTplt_Recipient</v>
+        <v>SHR_Scope_DlvrParcelTemplate_Recipient</v>
       </c>
       <c r="B8" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>SHR_PclRxTplt_Recipient</v>
+        <v>SHR_Scope_DlvrParcelTemplate_Recipient</v>
       </c>
       <c r="C8" s="20" t="str">
         <f>IF($D8="","",'#Scopes'!$A$4)</f>
-        <v>PclRxTplt</v>
+        <v>Scope_DlvrParcelTemplate</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="13"/>
@@ -1068,14 +1070,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.44140625" customWidth="1"/>
+    <col min="1" max="1" width="50.5546875" customWidth="1"/>
+    <col min="2" max="2" width="8" customWidth="1"/>
     <col min="3" max="3" width="15.109375" style="13" customWidth="1"/>
     <col min="4" max="4" width="32.33203125" style="13" customWidth="1"/>
     <col min="5" max="5" width="16.77734375" style="13" customWidth="1"/>
@@ -1084,10 +1086,10 @@
   <sheetData>
     <row r="1" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="22" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C1" s="15" t="s">
         <v>8</v>
@@ -1096,7 +1098,7 @@
         <v>9</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F1" s="9" t="s">
         <v>11</v>
@@ -1126,139 +1128,139 @@
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="str">
         <f>IF(OR($C3="",$D3=""),"",CONCATENATE("Obj_",$C3,"_",$D3))</f>
-        <v>Obj_PclTxTplt_Transportation need</v>
+        <v>Obj_Scope_SendParcelTemplate_Transportation need</v>
       </c>
       <c r="B3" s="16" t="str">
         <f t="shared" ref="B3" si="0">IF($A3="","",$A3)</f>
-        <v>Obj_PclTxTplt_Transportation need</v>
+        <v>Obj_Scope_SendParcelTemplate_Transportation need</v>
       </c>
       <c r="C3" s="14" t="str">
         <f>IF(AND($F3="",$D3=""),"",'#Scopes'!$A$3)</f>
-        <v>PclTxTplt</v>
+        <v>Scope_SendParcelTemplate</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>16</v>
       </c>
       <c r="F3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="str">
         <f t="shared" ref="A4:A9" si="1">IF(OR($C4="",$D4=""),"",CONCATENATE("Obj_",$C4,"_",$D4))</f>
-        <v>Obj_PclTxTplt_Transportation offer</v>
+        <v>Obj_Scope_SendParcelTemplate_Transportation offer</v>
       </c>
       <c r="B4" s="16" t="str">
         <f t="shared" ref="B4:B9" si="2">IF($A4="","",$A4)</f>
-        <v>Obj_PclTxTplt_Transportation offer</v>
+        <v>Obj_Scope_SendParcelTemplate_Transportation offer</v>
       </c>
       <c r="C4" s="14" t="str">
         <f>IF(AND($F4="",$D4=""),"",'#Scopes'!$A$3)</f>
-        <v>PclTxTplt</v>
+        <v>Scope_SendParcelTemplate</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>17</v>
       </c>
       <c r="F4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>Obj_PclTxTplt_Commit to pay</v>
+        <v>Obj_Scope_SendParcelTemplate_Commit to pay</v>
       </c>
       <c r="B5" s="16" t="str">
         <f t="shared" si="2"/>
-        <v>Obj_PclTxTplt_Commit to pay</v>
+        <v>Obj_Scope_SendParcelTemplate_Commit to pay</v>
       </c>
       <c r="C5" s="14" t="str">
         <f>IF(AND($F5="",$D5=""),"",'#Scopes'!$A$3)</f>
-        <v>PclTxTplt</v>
+        <v>Scope_SendParcelTemplate</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>17</v>
       </c>
       <c r="F5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>Obj_PclTxTplt_Parcel identifiability by Transporter</v>
+        <v>Obj_Scope_SendParcelTemplate_Parcel identifiability by Transporter</v>
       </c>
       <c r="B6" s="16" t="str">
         <f t="shared" si="2"/>
-        <v>Obj_PclTxTplt_Parcel identifiability by Transporter</v>
+        <v>Obj_Scope_SendParcelTemplate_Parcel identifiability by Transporter</v>
       </c>
       <c r="C6" s="14" t="str">
         <f>IF(AND($F6="",$D6=""),"",'#Scopes'!$A$3)</f>
-        <v>PclTxTplt</v>
+        <v>Scope_SendParcelTemplate</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>16</v>
       </c>
       <c r="F6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>Obj_PclRxTplt_Parcel delivery</v>
+        <v>Obj_Scope_DlvrParcelTemplate_Parcel delivery</v>
       </c>
       <c r="B8" s="16" t="str">
         <f t="shared" si="2"/>
-        <v>Obj_PclRxTplt_Parcel delivery</v>
+        <v>Obj_Scope_DlvrParcelTemplate_Parcel delivery</v>
       </c>
       <c r="C8" s="14" t="str">
         <f>IF(AND($F8="",$D8=""),"",'#Scopes'!$A$4)</f>
-        <v>PclRxTplt</v>
+        <v>Scope_DlvrParcelTemplate</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E8" s="13" t="s">
         <v>17</v>
       </c>
       <c r="F8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>Obj_PclRxTplt_Recipient signature</v>
+        <v>Obj_Scope_DlvrParcelTemplate_Recipient signature</v>
       </c>
       <c r="B9" s="16" t="str">
         <f t="shared" si="2"/>
-        <v>Obj_PclRxTplt_Recipient signature</v>
+        <v>Obj_Scope_DlvrParcelTemplate_Recipient signature</v>
       </c>
       <c r="C9" s="14" t="str">
         <f>IF(AND($F9="",$D9=""),"",'#Scopes'!$A$4)</f>
-        <v>PclRxTplt</v>
+        <v>Scope_DlvrParcelTemplate</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E9" s="13" t="s">
         <v>17</v>
       </c>
       <c r="F9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1272,7 +1274,7 @@
   <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1282,7 +1284,8 @@
     <col min="3" max="3" width="18.21875" style="10" customWidth="1"/>
     <col min="4" max="4" width="14.109375" style="10" customWidth="1"/>
     <col min="5" max="5" width="69.21875" style="12" customWidth="1"/>
-    <col min="6" max="7" width="13.77734375" style="11" customWidth="1"/>
+    <col min="6" max="6" width="13.77734375" style="10" customWidth="1"/>
+    <col min="7" max="7" width="13.77734375" style="11" customWidth="1"/>
     <col min="8" max="8" width="13.5546875" style="11" customWidth="1"/>
     <col min="9" max="21" width="13.77734375" style="11" customWidth="1"/>
     <col min="22" max="16384" width="8.88671875" style="11"/>
@@ -1305,7 +1308,7 @@
         <v>11</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
@@ -1340,7 +1343,7 @@
         <v>13</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
@@ -1358,14 +1361,14 @@
       <c r="T2" s="6"/>
       <c r="U2" s="6"/>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="str">
         <f>IF(OR($B3="",$C3=""),"",CONCATENATE("Var_",$B3,"_",$C3))</f>
-        <v>Var_PclTxTplt_Parcel</v>
+        <v>Var_Scope_SendParcelTemplate_Parcel</v>
       </c>
       <c r="B3" s="14" t="str">
         <f>IF(AND($E3="",$C3=""),"",'#Scopes'!$A$3)</f>
-        <v>PclTxTplt</v>
+        <v>Scope_SendParcelTemplate</v>
       </c>
       <c r="C3" s="13" t="s">
         <v>15</v>
@@ -1374,38 +1377,38 @@
         <v>16</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F3" s="7"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="str">
         <f>IF(OR($B4="",$C4=""),"",CONCATENATE("Var_",$B4,"_",$C4))</f>
-        <v>Var_PclTxTplt_Barcode</v>
+        <v>Var_Scope_SendParcelTemplate_Barcode</v>
       </c>
       <c r="B4" s="14" t="str">
         <f>IF(AND($E4="",$C4=""),"",'#Scopes'!$A$3)</f>
-        <v>PclTxTplt</v>
+        <v>Scope_SendParcelTemplate</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D4" s="13" t="s">
         <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H4" s="7"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" s="16" t="str">
         <f>IF(OR($B5="",$C5=""),"",CONCATENATE("Var_",$B5,"_",$C5))</f>
-        <v>Var_PclTxTplt_SenderAddress</v>
+        <v>Var_Scope_SendParcelTemplate_SenderAddress</v>
       </c>
       <c r="B5" s="14" t="str">
         <f>IF(AND($E5="",$C5=""),"",'#Scopes'!$A$3)</f>
-        <v>PclTxTplt</v>
+        <v>Scope_SendParcelTemplate</v>
       </c>
       <c r="C5" s="13" t="s">
         <v>20</v>
@@ -1414,45 +1417,45 @@
         <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" s="16" t="str">
         <f>IF(OR($B6="",$C6=""),"",CONCATENATE("Var_",$B6,"_",$C6))</f>
-        <v>Var_PclTxTplt_DeliveryAddress</v>
+        <v>Var_Scope_SendParcelTemplate_DeliveryAddress</v>
       </c>
       <c r="B6" s="14" t="str">
         <f>IF(AND($E6="",$C6=""),"",'#Scopes'!$A$3)</f>
-        <v>PclTxTplt</v>
+        <v>Scope_SendParcelTemplate</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D6" s="13" t="s">
         <v>16</v>
       </c>
       <c r="E6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" s="16" t="str">
         <f t="shared" ref="A7:A23" si="0">IF(OR($B7="",$C7=""),"",CONCATENATE("Var_",$B7,"_",$C7))</f>
-        <v>Var_PclTxTplt_Recipient</v>
+        <v>Var_Scope_SendParcelTemplate_Recipient</v>
       </c>
       <c r="B7" s="14" t="str">
         <f>IF(AND($E7="",$C7=""),"",'#Scopes'!$A$3)</f>
-        <v>PclTxTplt</v>
+        <v>Scope_SendParcelTemplate</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D7" s="13" t="s">
         <v>16</v>
       </c>
       <c r="E7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
@@ -1460,11 +1463,11 @@
     <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>Var_PclTxTplt_TransportationFee</v>
+        <v>Var_Scope_SendParcelTemplate_TransportationFee</v>
       </c>
       <c r="B8" s="14" t="str">
         <f>IF(AND($E8="",$C8=""),"",'#Scopes'!$A$3)</f>
-        <v>PclTxTplt</v>
+        <v>Scope_SendParcelTemplate</v>
       </c>
       <c r="C8" s="13" t="s">
         <v>21</v>
@@ -1473,9 +1476,9 @@
         <v>17</v>
       </c>
       <c r="E8" t="s">
-        <v>55</v>
-      </c>
-      <c r="F8" s="11">
+        <v>53</v>
+      </c>
+      <c r="F8" s="10">
         <v>2</v>
       </c>
       <c r="G8" s="7"/>
@@ -1484,31 +1487,31 @@
     <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>Var_PclTxTplt_Dimensions</v>
+        <v>Var_Scope_SendParcelTemplate_Dimensions</v>
       </c>
       <c r="B9" s="14" t="str">
         <f>IF(AND($E9="",$C9=""),"",'#Scopes'!$A$3)</f>
-        <v>PclTxTplt</v>
+        <v>Scope_SendParcelTemplate</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D9" s="10" t="s">
         <v>16</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="J9" s="7"/>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>Var_PclTxTplt_Weight</v>
+        <v>Var_Scope_SendParcelTemplate_Weight</v>
       </c>
       <c r="B10" s="14" t="str">
         <f>IF(AND($E10="",$C10=""),"",'#Scopes'!$A$3)</f>
-        <v>PclTxTplt</v>
+        <v>Scope_SendParcelTemplate</v>
       </c>
       <c r="C10" s="10" t="s">
         <v>22</v>
@@ -1517,7 +1520,7 @@
         <v>16</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.3">
@@ -1526,79 +1529,79 @@
     <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>Var_PclRxTplt_Barcode</v>
+        <v>Var_Scope_DlvrParcelTemplate_Barcode</v>
       </c>
       <c r="B12" s="14" t="str">
         <f>IF(AND($E12="",$C12=""),"",'#Scopes'!$A$4)</f>
-        <v>PclRxTplt</v>
+        <v>Scope_DlvrParcelTemplate</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D12" s="13" t="s">
         <v>17</v>
       </c>
       <c r="E12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>Var_PclRxTplt_DeliveryAddress</v>
+        <v>Var_Scope_DlvrParcelTemplate_DeliveryAddress</v>
       </c>
       <c r="B13" s="14" t="str">
         <f>IF(AND($E13="",$C13=""),"",'#Scopes'!$A$4)</f>
-        <v>PclRxTplt</v>
+        <v>Scope_DlvrParcelTemplate</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D13" s="13" t="s">
         <v>17</v>
       </c>
       <c r="E13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>Var_PclRxTplt_DeliveryReceipt</v>
+        <v>Var_Scope_DlvrParcelTemplate_DeliveryReceipt</v>
       </c>
       <c r="B14" s="14" t="str">
         <f>IF(AND($E14="",$C14=""),"",'#Scopes'!$A$4)</f>
-        <v>PclRxTplt</v>
+        <v>Scope_DlvrParcelTemplate</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D14" s="10" t="s">
         <v>17</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>Var_PclRxTplt_ReceiptSignature</v>
+        <v>Var_Scope_DlvrParcelTemplate_ReceiptSignature</v>
       </c>
       <c r="B15" s="14" t="str">
         <f>IF(AND($E15="",$C15=""),"",'#Scopes'!$A$4)</f>
-        <v>PclRxTplt</v>
+        <v>Scope_DlvrParcelTemplate</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="F15" s="11">
+        <v>62</v>
+      </c>
+      <c r="F15" s="10">
         <v>2</v>
       </c>
     </row>
@@ -1704,10 +1707,10 @@
   <sheetData>
     <row r="1" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
@@ -1733,10 +1736,10 @@
     </row>
     <row r="2" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
@@ -1762,34 +1765,34 @@
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>